<commit_message>
Processos de preenchimento de cabeçalho no inicio do bot
</commit_message>
<xml_diff>
--- a/planilha_reembolso_branco.xlsx
+++ b/planilha_reembolso_branco.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yellows\bot_planilha_de_custos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0D2640-5C1C-4447-A78A-92ACB4D66A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08682726-059E-45E0-9140-42E2016ED0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>RELATÓRIO DE DESPESAS - REEMBOLSO</t>
   </si>
@@ -291,12 +291,6 @@
   </si>
   <si>
     <t xml:space="preserve">DAVI MARIM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rubsney Nascimento </t>
-  </si>
-  <si>
-    <t>Nubank</t>
   </si>
   <si>
     <t xml:space="preserve">       ITO1 FI 003-03 - 3ª ED 06/11/2024</t>
@@ -1349,16 +1343,55 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="6" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1392,45 +1425,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="6" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="4" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="4" fillId="5" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1692,7 +1686,7 @@
   <dimension ref="B1:J1025"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1712,39 +1706,37 @@
   <sheetData>
     <row r="1" spans="2:10" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="65"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="84"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="75" t="s">
+      <c r="B3" s="85"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="76"/>
+      <c r="F3" s="95"/>
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="78"/>
-      <c r="J3" s="76"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="95"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="71"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1752,14 +1744,14 @@
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="81"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="69"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="90"/>
       <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
@@ -1767,54 +1759,52 @@
       <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="82" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="81"/>
     </row>
     <row r="6" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="79" t="s">
+      <c r="B6" s="88"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="80" t="s">
+      <c r="F6" s="99" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="59"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="81"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="72"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="81"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="100"/>
       <c r="G7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="59"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="81"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="72"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
@@ -2250,25 +2240,25 @@
       <c r="E46" s="21"/>
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
-      <c r="H46" s="83">
+      <c r="H46" s="69">
         <f>SUM(I10:I45)</f>
         <v>0</v>
       </c>
-      <c r="I46" s="84"/>
+      <c r="I46" s="70"/>
       <c r="J46" s="22"/>
     </row>
     <row r="47" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="60" t="s">
+      <c r="B47" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="61"/>
-      <c r="D47" s="61"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="61"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="61"/>
-      <c r="I47" s="61"/>
-      <c r="J47" s="62"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="71"/>
+      <c r="H47" s="71"/>
+      <c r="I47" s="71"/>
+      <c r="J47" s="72"/>
     </row>
     <row r="48" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="23"/>
@@ -2282,27 +2272,27 @@
       <c r="J48" s="25"/>
     </row>
     <row r="49" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="85" t="s">
+      <c r="B49" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="86"/>
-      <c r="D49" s="87"/>
+      <c r="C49" s="74"/>
+      <c r="D49" s="75"/>
       <c r="E49" s="24"/>
-      <c r="F49" s="88" t="s">
+      <c r="F49" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="G49" s="87"/>
+      <c r="G49" s="75"/>
       <c r="H49" s="26"/>
-      <c r="I49" s="89"/>
-      <c r="J49" s="90"/>
+      <c r="I49" s="77"/>
+      <c r="J49" s="78"/>
     </row>
     <row r="50" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="91" t="s">
+      <c r="B50" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="92"/>
+      <c r="C50" s="63"/>
       <c r="D50" s="27">
-        <f>SUMIF($D$11:$D$45,B50,$I$11:$I$45)</f>
+        <f t="shared" ref="D50:D56" si="0">SUMIF($D$11:$D$45,B50,$I$11:$I$45)</f>
         <v>0</v>
       </c>
       <c r="E50" s="28"/>
@@ -2318,12 +2308,12 @@
       <c r="J50" s="31"/>
     </row>
     <row r="51" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="93" t="s">
+      <c r="B51" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="92"/>
+      <c r="C51" s="63"/>
       <c r="D51" s="32">
-        <f>SUMIF($D$11:$D$45,B51,$I$11:$I$45)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E51" s="24"/>
@@ -2331,7 +2321,7 @@
         <v>27</v>
       </c>
       <c r="G51" s="32">
-        <f>SUMIF($C$11:$C$45,F51,$I$11:$I$45)</f>
+        <f t="shared" ref="G51:G59" si="1">SUMIF($C$11:$C$45,F51,$I$11:$I$45)</f>
         <v>0</v>
       </c>
       <c r="H51" s="26"/>
@@ -2339,12 +2329,12 @@
       <c r="J51" s="25"/>
     </row>
     <row r="52" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="93" t="s">
+      <c r="B52" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="92"/>
+      <c r="C52" s="63"/>
       <c r="D52" s="32">
-        <f>SUMIF($D$11:$D$45,B52,$I$11:$I$45)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E52" s="24"/>
@@ -2352,7 +2342,7 @@
         <v>29</v>
       </c>
       <c r="G52" s="32">
-        <f>SUMIF($C$11:$C$45,F52,$I$11:$I$45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H52" s="26"/>
@@ -2360,12 +2350,12 @@
       <c r="J52" s="25"/>
     </row>
     <row r="53" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="93" t="s">
+      <c r="B53" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="92"/>
+      <c r="C53" s="63"/>
       <c r="D53" s="32">
-        <f>SUMIF($D$11:$D$45,B53,$I$11:$I$45)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E53" s="24"/>
@@ -2373,7 +2363,7 @@
         <v>31</v>
       </c>
       <c r="G53" s="32">
-        <f>SUMIF($C$11:$C$45,F53,$I$11:$I$45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H53" s="26"/>
@@ -2381,12 +2371,12 @@
       <c r="J53" s="25"/>
     </row>
     <row r="54" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="93" t="s">
+      <c r="B54" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="92"/>
+      <c r="C54" s="63"/>
       <c r="D54" s="32">
-        <f>SUMIF($D$11:$D$45,B54,$I$11:$I$45)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E54" s="24"/>
@@ -2394,7 +2384,7 @@
         <v>33</v>
       </c>
       <c r="G54" s="32">
-        <f>SUMIF($C$11:$C$45,F54,$I$11:$I$45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H54" s="26"/>
@@ -2402,12 +2392,12 @@
       <c r="J54" s="25"/>
     </row>
     <row r="55" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="93" t="s">
+      <c r="B55" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="C55" s="92"/>
+      <c r="C55" s="63"/>
       <c r="D55" s="32">
-        <f>SUMIF($D$11:$D$45,B55,$I$11:$I$45)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E55" s="24"/>
@@ -2415,7 +2405,7 @@
         <v>34</v>
       </c>
       <c r="G55" s="32">
-        <f>SUMIF($C$11:$C$45,F55,$I$11:$I$45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H55" s="26"/>
@@ -2423,12 +2413,12 @@
       <c r="J55" s="25"/>
     </row>
     <row r="56" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="93" t="s">
+      <c r="B56" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="92"/>
+      <c r="C56" s="63"/>
       <c r="D56" s="32">
-        <f>SUMIF($D$11:$D$45,B56,$I$11:$I$45)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E56" s="24"/>
@@ -2436,7 +2426,7 @@
         <v>36</v>
       </c>
       <c r="G56" s="35">
-        <f>SUMIF($C$11:$C$45,F56,$I$11:$I$45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H56" s="26"/>
@@ -2444,10 +2434,10 @@
       <c r="J56" s="25"/>
     </row>
     <row r="57" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="93" t="s">
+      <c r="B57" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="92"/>
+      <c r="C57" s="63"/>
       <c r="D57" s="32">
         <f>SUMIF($D$11:$D$45,#REF!,$I$11:$I$45)</f>
         <v>0</v>
@@ -2457,7 +2447,7 @@
         <v>33</v>
       </c>
       <c r="G57" s="32">
-        <f>SUMIF($C$11:$C$45,F57,$I$11:$I$45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H57" s="26"/>
@@ -2465,10 +2455,10 @@
       <c r="J57" s="25"/>
     </row>
     <row r="58" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="93" t="s">
+      <c r="B58" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C58" s="92"/>
+      <c r="C58" s="63"/>
       <c r="D58" s="32">
         <f>SUMIF($D$11:$D$45,B58,$I$11:$I$45)</f>
         <v>0</v>
@@ -2478,7 +2468,7 @@
         <v>33</v>
       </c>
       <c r="G58" s="32">
-        <f>SUMIF($C$11:$C$45,F58,$I$11:$I$45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H58" s="26"/>
@@ -2486,10 +2476,10 @@
       <c r="J58" s="25"/>
     </row>
     <row r="59" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="93" t="s">
+      <c r="B59" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="C59" s="92"/>
+      <c r="C59" s="63"/>
       <c r="D59" s="32">
         <f>SUMIF($D$11:$D$45,B59,$I$11:$I$45)</f>
         <v>0</v>
@@ -2499,7 +2489,7 @@
         <v>40</v>
       </c>
       <c r="G59" s="35">
-        <f>SUMIF($C$11:$C$45,F59,$I$11:$I$45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H59" s="26"/>
@@ -2507,10 +2497,10 @@
       <c r="J59" s="25"/>
     </row>
     <row r="60" spans="2:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="98" t="s">
+      <c r="B60" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C60" s="99"/>
+      <c r="C60" s="65"/>
       <c r="D60" s="37">
         <f>SUM(D50:D59)</f>
         <v>0</v>
@@ -2550,10 +2540,10 @@
       <c r="J62" s="25"/>
     </row>
     <row r="63" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="60" t="s">
+      <c r="B63" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="C63" s="100"/>
+      <c r="C63" s="67"/>
       <c r="D63" s="41"/>
       <c r="E63" s="41"/>
       <c r="F63" s="41"/>
@@ -2574,11 +2564,11 @@
       <c r="J64" s="25"/>
     </row>
     <row r="65" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="94" t="s">
+      <c r="B65" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C65" s="95"/>
-      <c r="D65" s="101" t="s">
+      <c r="C65" s="59"/>
+      <c r="D65" s="57" t="s">
         <v>44</v>
       </c>
       <c r="E65" s="43"/>
@@ -2589,10 +2579,10 @@
       <c r="J65" s="25"/>
     </row>
     <row r="66" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="94" t="s">
+      <c r="B66" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="C66" s="95"/>
+      <c r="C66" s="59"/>
       <c r="D66" s="24"/>
       <c r="E66" s="24"/>
       <c r="F66" s="24"/>
@@ -2602,10 +2592,10 @@
       <c r="J66" s="25"/>
     </row>
     <row r="67" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="94" t="s">
+      <c r="B67" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="C67" s="95"/>
+      <c r="C67" s="59"/>
       <c r="D67" s="44"/>
       <c r="E67" s="24"/>
       <c r="F67" s="24"/>
@@ -2637,10 +2627,10 @@
       <c r="J69" s="50"/>
     </row>
     <row r="70" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="94" t="s">
+      <c r="B70" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="C70" s="95"/>
+      <c r="C70" s="59"/>
       <c r="D70" s="51" t="s">
         <v>48</v>
       </c>
@@ -2652,10 +2642,10 @@
       <c r="J70" s="25"/>
     </row>
     <row r="71" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="94" t="s">
+      <c r="B71" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="C71" s="95"/>
+      <c r="C71" s="59"/>
       <c r="D71" s="24"/>
       <c r="E71" s="24"/>
       <c r="F71" s="24"/>
@@ -2665,10 +2655,10 @@
       <c r="J71" s="25"/>
     </row>
     <row r="72" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="94" t="s">
+      <c r="B72" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="C72" s="95"/>
+      <c r="C72" s="59"/>
       <c r="D72" s="24"/>
       <c r="E72" s="24"/>
       <c r="F72" s="24"/>
@@ -2689,10 +2679,10 @@
       <c r="J73" s="25"/>
     </row>
     <row r="74" spans="2:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="96" t="s">
-        <v>51</v>
-      </c>
-      <c r="C74" s="97"/>
+      <c r="B74" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="61"/>
       <c r="D74" s="53"/>
       <c r="E74" s="53"/>
       <c r="F74" s="53"/>
@@ -3654,30 +3644,6 @@
     <row r="1025" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="B47:J47"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="I49:J49"/>
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B2:J2"/>
@@ -3689,6 +3655,30 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="B47:J47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D11:D12 D14:D45" xr:uid="{00000000-0002-0000-0000-000001000000}">

</xml_diff>